<commit_message>
better headings in the colouring and format
</commit_message>
<xml_diff>
--- a/Project Management/BurnDown Charts/BurnDown Chart Sprint 4.xlsx
+++ b/Project Management/BurnDown Charts/BurnDown Chart Sprint 4.xlsx
@@ -77,12 +77,30 @@
     </font>
     <font/>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF93C47D"/>
+        <bgColor rgb="FF93C47D"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEFEFEF"/>
+        <bgColor rgb="FFEFEFEF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -91,14 +109,17 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -123,53 +144,53 @@
     <col customWidth="1" min="1" max="1" width="36.29"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="33.0" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added the resulting categories
</commit_message>
<xml_diff>
--- a/Project Management/BurnDown Charts/BurnDown Chart Sprint 4.xlsx
+++ b/Project Management/BurnDown Charts/BurnDown Chart Sprint 4.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Stories for the Sprint</t>
   </si>
@@ -59,13 +59,25 @@
   </si>
   <si>
     <t>Day 14 (Hours)</t>
+  </si>
+  <si>
+    <t>Remaining Effort</t>
+  </si>
+  <si>
+    <t>Ideal Burndown</t>
+  </si>
+  <si>
+    <t>Stories Remaining</t>
+  </si>
+  <si>
+    <t>Stories Completed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -76,6 +88,9 @@
       <sz val="14.0"/>
     </font>
     <font/>
+    <font>
+      <sz val="12.0"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -109,7 +124,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -120,6 +135,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -194,6 +212,26 @@
         <v>15</v>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
maybe the excel into a more table look
</commit_message>
<xml_diff>
--- a/Project Management/BurnDown Charts/BurnDown Chart Sprint 4.xlsx
+++ b/Project Management/BurnDown Charts/BurnDown Chart Sprint 4.xlsx
@@ -118,26 +118,41 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border/>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -212,25 +227,427 @@
         <v>15</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+    </row>
     <row r="21">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="5" t="s">
         <v>16</v>
       </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
     </row>
     <row r="22">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
     </row>
     <row r="23">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
     </row>
     <row r="24">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="5" t="s">
         <v>19</v>
       </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>